<commit_message>
More Syria public plicy being phased
</commit_message>
<xml_diff>
--- a/src/brt_google_mobility/acaps_missing.xlsx
+++ b/src/brt_google_mobility/acaps_missing.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="43">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -103,12 +103,15 @@
     <t xml:space="preserve">Nationwide curfew lifted. The Syrian government announced on Monday, May 25, the lifting of the nationwide curfew as of Tuesday, May 26, originally in place to curb the spread of the coronavirus disease (COVID-19). The curfew, originally imposed on Wednesday, March 25, ran from 18:00 to 06:00 (local time).  Authorities have also eased lockdown restrictions on shops and other businesses, which will now be allowed to remain open from 08:00 to 19:00 (local time). Authorities stated on May 25 that a curfew could be re-introduced in the future depending on developments relating to the pandemic.</t>
   </si>
   <si>
+    <t xml:space="preserve">Garda World</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Government</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.garda.com/crisis24/news-alerts/345376/syria-syrian-authorities-to-lift-curfew-and-allow-inter-provincial-travel-as-of-may-26-update-4</t>
   </si>
   <si>
-    <t xml:space="preserve">Government</t>
-  </si>
-  <si>
     <t xml:space="preserve">Movement between provinces/public transport resume. As part of the new easing of measures announced, movement between provinces will be allowed and public transport will be operating on May 26. As passenger flights into and out of the country remain halted, authorities have now also announced the ceasing of repatriation flights into Syria as they look to try and reduce the number of potential new cases in the country.</t>
   </si>
   <si>
@@ -128,21 +131,41 @@
   </si>
   <si>
     <t xml:space="preserve">Limit public gatherings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Religious Endowments (Awqaf) Ministry announced on Sunday that prayers for funerals have been suspended in mosques in Damascus and its countryside until further notice as a part of the preventive measures taken to prevent the spread of the Coronavirus (COVID-19) in the two provinces.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Syrian Arab News Agency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://sana.sy/en/?p=198341</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OCHA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://reliefweb.int/sites/reliefweb.int/files/resources/final_draft_covid-19_update_no._9.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -164,16 +187,19 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Liberation Mono;Courier New;DejaVu Sans Mono"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -218,7 +244,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -240,6 +266,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -260,10 +298,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N14" activeCellId="0" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -370,7 +408,7 @@
         <v>28</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="Q2" s="4" t="n">
         <v>43977</v>
@@ -406,7 +444,7 @@
         <v>25</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M3" s="4" t="n">
         <v>43977</v>
@@ -418,7 +456,7 @@
         <v>28</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="Q3" s="4" t="n">
         <v>43977</v>
@@ -448,13 +486,13 @@
         <v>23</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>25</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M4" s="4" t="n">
         <v>43977</v>
@@ -466,7 +504,7 @@
         <v>28</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="Q4" s="4" t="n">
         <v>43977</v>
@@ -495,13 +533,13 @@
         <v>23</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>25</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M5" s="4" t="n">
         <v>43977</v>
@@ -513,7 +551,7 @@
         <v>28</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="Q5" s="4" t="n">
         <v>43977</v>
@@ -536,19 +574,19 @@
         <v>21</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>35</v>
+      <c r="I6" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>25</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M6" s="4" t="n">
         <v>43977</v>
@@ -560,10 +598,104 @@
         <v>28</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="Q6" s="4" t="n">
         <v>43977</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="51.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="M7" s="4" t="n">
+        <v>44038</v>
+      </c>
+      <c r="N7" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="O7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q7" s="8" t="n">
+        <v>44008</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="M8" s="4" t="n">
+        <v>44059</v>
+      </c>
+      <c r="N8" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="O8" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="P8" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q8" s="8" t="n">
+        <v>44008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>